<commit_message>
change in serial squence
</commit_message>
<xml_diff>
--- a/serial readings .xlsx
+++ b/serial readings .xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>y angle</t>
   </si>
@@ -104,7 +104,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -115,6 +115,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -130,6 +133,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -412,19 +416,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="10" max="10" width="10" customWidth="1"/>
     <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="12" max="13" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -432,136 +437,170 @@
         <f>A1+1</f>
         <v>2</v>
       </c>
-      <c r="C1" s="5">
+      <c r="C1" s="4">
         <f t="shared" ref="C1:L1" si="0">B1+1</f>
         <v>3</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E1" s="4">
+      <c r="E1" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G1" s="5">
+      <c r="G1" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="H1" s="5">
+      <c r="H1" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I1" s="5">
+      <c r="I1" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="J1" s="5">
+      <c r="J1" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K1" s="4">
+      <c r="K1" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="L1" s="5">
+      <c r="L1" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="6" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="5" t="s">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D5" s="8" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1</v>
       </c>
       <c r="B7" s="2">
+        <f>A7+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="6">
+        <f t="shared" ref="C7:M7" si="1">B7+1</f>
         <v>3</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="6">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="5">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="5">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="5">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="5">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="6">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="6">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
+      <c r="K7" s="6">
+        <f>J7+1</f>
+        <v>11</v>
+      </c>
+      <c r="L7" s="5">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="M7" s="6">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="M8" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="I8:K8"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="G2:J2"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
organiztion and UART codes
</commit_message>
<xml_diff>
--- a/serial readings .xlsx
+++ b/serial readings .xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -124,6 +125,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -133,7 +135,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -418,7 +419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -479,22 +480,22 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="7" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
       <c r="K2" s="6" t="s">
         <v>3</v>
       </c>
@@ -503,11 +504,11 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -563,23 +564,23 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="8" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="7" t="s">
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
       <c r="L8" s="2" t="s">
         <v>3</v>
       </c>
@@ -588,9 +589,9 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>